<commit_message>
Did a lot of drawings.
</commit_message>
<xml_diff>
--- a/Procurement/BOM.xlsx
+++ b/Procurement/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FYP\Procurement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35DA4FF-95C2-4E3F-838F-45B2CAF5818E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E60B43-76DD-47DD-BDF8-C6BF453CCD0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,9 +38,6 @@
     <t>Motor</t>
   </si>
   <si>
-    <t>172:1 Metal Gearmotor 25Dx71L mm HP 6V with 48 CPR Encoder</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -63,9 +62,6 @@
     <t>Info</t>
   </si>
   <si>
-    <t>56RPM max, 2.45 Nm</t>
-  </si>
-  <si>
     <t>Motor Bracket</t>
   </si>
   <si>
@@ -78,9 +74,6 @@
     <t>MEC-30197</t>
   </si>
   <si>
-    <t>SKU-005617</t>
-  </si>
-  <si>
     <t>It’s a bracket.</t>
   </si>
   <si>
@@ -127,6 +120,15 @@
   </si>
   <si>
     <t>USD</t>
+  </si>
+  <si>
+    <t>99:1 Metal Gearmotor 25Dx69L mm HP 12V with 48 CPR Encoder</t>
+  </si>
+  <si>
+    <t>SKU-005518</t>
+  </si>
+  <si>
+    <t>100RPM, 2.11 Nm, 12V 5A</t>
   </si>
 </sst>
 </file>
@@ -475,83 +477,83 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>4808</v>
+        <v>4847</v>
       </c>
       <c r="D3">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
       <c r="C6">
         <v>2676</v>
@@ -560,26 +562,26 @@
         <v>10</v>
       </c>
       <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
       </c>
       <c r="C9">
         <v>1451</v>
@@ -588,26 +590,26 @@
         <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>634084</v>
@@ -616,25 +618,25 @@
         <v>3.1</v>
       </c>
       <c r="E12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12">
         <f>C12</f>
         <v>634084</v>
       </c>
       <c r="G12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C13">
         <v>625118</v>
@@ -643,25 +645,25 @@
         <v>4.99</v>
       </c>
       <c r="E13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F13">
         <f t="shared" ref="F13:F14" si="0">C13</f>
         <v>625118</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>625049</v>
@@ -670,30 +672,30 @@
         <v>4.99</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
         <v>625049</v>
       </c>
       <c r="G14" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
         <v>28</v>
       </c>
-      <c r="M14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17">
         <v>535198</v>
@@ -702,24 +704,24 @@
         <v>2.89</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F17">
         <v>535198</v>
       </c>
       <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="M17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C18">
         <v>535020</v>
@@ -728,20 +730,20 @@
         <v>2.19</v>
       </c>
       <c r="E18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F18">
         <v>535020</v>
       </c>
       <c r="G18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>